<commit_message>
thesis edits and model changes
</commit_message>
<xml_diff>
--- a/Compiled Report/Original Data/USD to Euro Conversion Avg by Year.xlsx
+++ b/Compiled Report/Original Data/USD to Euro Conversion Avg by Year.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/benasmith/Desktop/Research Proj/Pharma Proj/Cleaned Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/benasmith/Desktop/Research Proj/Pharma Proj/BenaSmithThesis/Compiled Report/Original Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFEB97C7-1DA4-0F47-BA47-4655873E425B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D59991D8-FDE3-7149-8B82-A097FB8FA805}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16180" xr2:uid="{41925F0C-8D21-FF42-ADEF-A09C94C01B74}"/>
   </bookViews>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Year</t>
   </si>
@@ -77,12 +77,15 @@
   <si>
     <t>Average Closing Price</t>
   </si>
+  <si>
+    <t>https://www.macrotrends.net/2548/euro-dollar-exchange-rate-historical-chart</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -115,12 +118,6 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -142,13 +139,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="10" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="10" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -504,10 +500,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE7FEBE8-23F8-904A-8550-856297019D41}">
-  <dimension ref="A1:G26"/>
+  <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -516,7 +512,7 @@
     <col min="7" max="7" width="20.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -535,11 +531,14 @@
       <c r="F1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" ht="20" x14ac:dyDescent="0.2">
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="20" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>2024</v>
       </c>
@@ -562,7 +561,7 @@
         <v>-1.9599999999999999E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="20" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" ht="20" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>2023</v>
       </c>
@@ -585,7 +584,7 @@
         <v>3.0599999999999999E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="20" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" ht="20" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>2022</v>
       </c>
@@ -608,7 +607,7 @@
         <v>-5.6599999999999998E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="20" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" ht="20" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>2021</v>
       </c>
@@ -631,7 +630,7 @@
         <v>-6.9199999999999998E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="20" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" ht="20" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>2020</v>
       </c>
@@ -654,7 +653,7 @@
         <v>8.8599999999999998E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="20" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" ht="20" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>2019</v>
       </c>
@@ -677,7 +676,7 @@
         <v>-2.2599999999999999E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="20" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" ht="20" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>2018</v>
       </c>
@@ -700,7 +699,7 @@
         <v>-4.36E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="20" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" ht="20" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>2017</v>
       </c>
@@ -723,7 +722,7 @@
         <v>0.14149999999999999</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="20" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" ht="20" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>2016</v>
       </c>
@@ -746,7 +745,7 @@
         <v>-3.1800000000000002E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="20" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" ht="20" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>2015</v>
       </c>
@@ -769,7 +768,7 @@
         <v>-0.1021</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="20" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" ht="20" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>2014</v>
       </c>
@@ -792,7 +791,7 @@
         <v>-0.1202</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="20" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" ht="20" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>2013</v>
       </c>
@@ -815,7 +814,7 @@
         <v>4.2599999999999999E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="20" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" ht="20" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>2012</v>
       </c>
@@ -838,7 +837,7 @@
         <v>1.9199999999999998E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="20" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" ht="20" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>2011</v>
       </c>
@@ -861,7 +860,7 @@
         <v>-3.2000000000000001E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="20" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" ht="20" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>2010</v>
       </c>

</xml_diff>